<commit_message>
fix Police Letter Template
</commit_message>
<xml_diff>
--- a/Raw Input Data/Template V2/PoliceLetter V2.xlsx
+++ b/Raw Input Data/Template V2/PoliceLetter V2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\hase-scripts\Raw Input Data\Template V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B710EB-5C98-4AD6-A96D-BEF9130A69AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9806C5-AAC9-48F2-BB7D-26F7BFF8A216}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="6690" windowWidth="29040" windowHeight="15720" tabRatio="859" activeTab="4" xr2:uid="{87512554-1306-F949-B1A5-DEDDB9062EFE}"/>
   </bookViews>
@@ -524,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -541,18 +541,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -891,7 +880,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07795220-ADDB-144F-9DAC-25D43AE85E71}">
-  <dimension ref="A1:Z24"/>
+  <dimension ref="A1:U24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
@@ -903,7 +892,7 @@
     <col min="2" max="2" width="27.875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -911,178 +900,164 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="10"/>
-      <c r="V2" s="8"/>
-      <c r="W2" s="8"/>
-      <c r="X2" s="8"/>
-      <c r="Y2" s="8"/>
-      <c r="Z2" s="8"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="P2" s="8"/>
+      <c r="U2" s="2"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="1" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="1" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" t="s">
         <v>101</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" t="s">
         <v>116</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" t="s">
         <v>117</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B15"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="8"/>
+      <c r="B16"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="8"/>
+      <c r="B17"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18"/>
     </row>
     <row r="19" spans="1:2" ht="173.25" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="2" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1090,7 +1065,7 @@
       <c r="A20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1098,13 +1073,13 @@
       <c r="A21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B21" s="8"/>
+      <c r="B21"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1112,7 +1087,7 @@
       <c r="A23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" t="s">
         <v>110</v>
       </c>
     </row>
@@ -1120,7 +1095,7 @@
       <c r="A24" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1177,7 +1152,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D9541C9-59CB-5C4B-8F3D-6BA72A7B78FE}">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F7"/>
@@ -1189,7 +1164,6 @@
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11" style="12"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -1205,25 +1179,25 @@
       <c r="D1" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" t="s">
         <v>122</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" t="s">
         <v>120</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" t="s">
         <v>123</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" t="s">
         <v>124</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="6" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1231,193 +1205,175 @@
       <c r="A2">
         <v>28</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="16">
+      <c r="C2" s="9">
         <v>100000</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" t="s">
         <v>125</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="10">
         <v>1</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" t="s">
         <v>132</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="K2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3">
         <v>28</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="16">
+      <c r="C3" s="9">
         <v>100000</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" t="s">
         <v>114</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" t="s">
         <v>126</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="17">
+      <c r="G3" s="10">
         <v>2</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" t="s">
         <v>132</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4">
         <v>28</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="16">
+      <c r="C4" s="9">
         <v>100000</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" t="s">
         <v>114</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" t="s">
         <v>127</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="10">
         <v>2</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" t="s">
         <v>132</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5">
         <v>28</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C5" s="16">
+      <c r="C5" s="9">
         <v>100000</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" t="s">
         <v>114</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5">
         <v>10</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" t="s">
         <v>64</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="10">
         <v>3</v>
       </c>
-      <c r="J5" s="12" t="s">
+      <c r="J5" t="s">
         <v>132</v>
       </c>
-      <c r="K5" s="12" t="s">
+      <c r="K5" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6">
         <v>28</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="9">
         <v>100000</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" t="s">
         <v>114</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" t="s">
         <v>128</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="10">
         <v>3</v>
       </c>
-      <c r="J6" s="12" t="s">
+      <c r="J6" t="s">
         <v>132</v>
       </c>
-      <c r="K6" s="12" t="s">
+      <c r="K6" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7">
         <v>28</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="9">
         <v>100000</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" t="s">
         <v>129</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="10">
         <v>4</v>
       </c>
-      <c r="J7" s="12" t="s">
+      <c r="J7" t="s">
         <v>132</v>
       </c>
-      <c r="K7" s="12" t="s">
+      <c r="K7" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1497,7 +1453,7 @@
     <col min="2" max="2" width="58.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:2" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2" ht="157.5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="str">
         <f>"&lt;Template_PoliceInvestigationTeam&gt;"&amp;'PoliceLetter-Params'!B2&amp;"&lt;/Template_PoliceInvestigationTeam&gt;"&amp;CHAR(10)&amp;"&lt;Template_PoliceForceDistrict&gt;"&amp;'PoliceLetter-Params'!B3&amp;"&lt;/Template_PoliceForceDistrict&gt;"&amp;CHAR(10)&amp;"&lt;Template_PITLocationBuilding&gt;"&amp;'PoliceLetter-Params'!B4&amp;"&lt;/Template_PITLocationBuilding&gt;"&amp;CHAR(10)&amp;"&lt;Template_PITLocationAddressLine&gt;"&amp;'PoliceLetter-Params'!B5&amp;"&lt;/Template_PITLocationAddressLine&gt;"&amp;CHAR(10)&amp;"&lt;Template_PITLocationDistrict&gt;"&amp;'PoliceLetter-Params'!B6&amp;"&lt;/Template_PITLocationDistrict&gt;"</f>
         <v>&lt;Template_PoliceInvestigationTeam&gt;District Investigation Team 7&lt;/Template_PoliceInvestigationTeam&gt;
@@ -1519,13 +1475,13 @@
         <v>&lt;tr&gt;&lt;th rowspan='3'&gt;FPS Proxy Type:&lt;/th&gt;&lt;td colspan='2'&gt; - [ ] Proxy ID&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='2'&gt; - [ ] Mobile Number&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='2'&gt; - [ ] E-mail&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="3" spans="2:2" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" ht="63" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="str">
         <f>IF('PoliceLetter-Params'!B12 = "Y", B2&amp;"&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B16&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;'PoliceLetter-Params'!B16&amp;"&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B17&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;'PoliceLetter-Params'!B17&amp;"&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B18&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;'PoliceLetter-Params'!B18&amp;"&lt;/td&gt;&lt;/tr&gt;","&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B19&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;"&lt;Template_AccountName&gt;"&amp;'PoliceLetter-Params'!B13&amp;"&lt;/Template_AccountName&gt;"&amp;"&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B20&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;'PoliceLetter-Params'!B14&amp;"&lt;/td&gt;&lt;/tr&gt;")</f>
         <v>&lt;tr&gt;&lt;th&gt;Account Name:&lt;/th&gt;&lt;td colspan='2'&gt;&lt;Template_AccountName&gt;CHAN TAI MAN &lt;/Template_AccountName&gt;&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Account Number:&lt;/th&gt;&lt;td colspan='2'&gt;111-111111-101 &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
     </row>
-    <row r="4" spans="2:2" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" ht="141.75" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="str" cm="1">
         <f t="array" ref="B4">_xlfn.LET(
   _xlpm.header, "&lt;tr&gt;&lt;th colspan='3'&gt;" &amp; 'PoliceLetter-Template'!B33 &amp; "&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;th&gt;" &amp; 'PoliceLetter-Template'!B34 &amp; "&lt;/th&gt;&lt;th&gt;" &amp; 'PoliceLetter-Template'!B35 &amp; "&lt;/th&gt;&lt;th&gt;" &amp; 'PoliceLetter-Template'!B36 &amp; "&lt;/th&gt;&lt;/tr&gt;",
@@ -1601,48 +1557,49 @@
   _xlpm.table_start, "&lt;table&gt;",
   _xlpm.header, "&lt;thead&gt;&lt;tr&gt;&lt;th colspan='3'&gt;" &amp; 'PoliceLetter-Template'!B11 &amp; "&lt;/th&gt;&lt;/tr&gt;&lt;/thead&gt;",
   _xlpm.tbody_start, "&lt;tbody&gt;",
+  _xlpm.unique_suspects, _xlfn.UNIQUE(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!G2:G100, 'PoliceLetter-Txn-Details'!G2:G100&lt;&gt;"")),
   _xlpm.make_account_table, _xlfn.LAMBDA(_xlpm.col_num,
     _xlfn.LET(
       _xlpm.account_name, INDEX('PoliceLetter-Params'!B13:U13, 1, _xlpm.col_num),
       _xlpm.account_number, INDEX('PoliceLetter-Params'!B14:U14, 1, _xlpm.col_num),
-      _xlpm.suspect_num, _xlpm.col_num,
+      _xlpm.suspect_num, INDEX(_xlpm.unique_suspects, _xlpm.col_num),
       _xlpm.account_detail, IF('PoliceLetter-Params'!B12 = "Y",
         B2&amp;"&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B16&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;'PoliceLetter-Params'!B16&amp;"&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B17&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;'PoliceLetter-Params'!B17&amp;"&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B18&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;'PoliceLetter-Params'!B18&amp;"&lt;/td&gt;&lt;/tr&gt;",
         "&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B19&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;"&lt;Template_Suspect"&amp;_xlpm.suspect_num&amp;"_Name&gt;"&amp;_xlpm.account_name&amp;"&lt;/Template_Suspect"&amp;_xlpm.suspect_num&amp;"_Name&gt;"&amp;"&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;"&amp;'PoliceLetter-Template'!B20&amp;"&lt;/th&gt;&lt;td colspan='2'&gt;"&amp;"&lt;Template_Suspect"&amp;_xlpm.suspect_num&amp;"_AccountNumber&gt;"&amp;_xlpm.account_number&amp;"&lt;/Template_Suspect"&amp;_xlpm.suspect_num&amp;"_AccountNumber&gt;"&amp;"&lt;/td&gt;&lt;/tr&gt;"
       ),
       _xlpm.transactions_rows, _xlfn.LET(
         _xlpm.header, "&lt;tr&gt;&lt;th colspan='3'&gt;" &amp; 'PoliceLetter-Template'!B33 &amp; "&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;" &amp; 'PoliceLetter-Template'!B34 &amp; "&lt;/th&gt;&lt;th&gt;" &amp; 'PoliceLetter-Template'!B35 &amp; "&lt;/th&gt;&lt;th&gt;" &amp; 'PoliceLetter-Template'!B36 &amp; "&lt;/th&gt;&lt;/tr&gt;",
-        _xlpm.filtered_txns, _xlfn._xlws.FILTER(
-          'PoliceLetter-Txn-Details'!B2:D100,
-          ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num),
-          "No Transaction"
-        ),
-        _xlpm.Ecol, _xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!E2:E100, ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num)),
-        _xlpm.Fcol, _xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!F2:F100, ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num)),
-        _xlpm.Hcol, _xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!H2:H100, ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num)),
-        _xlpm.Icol, _xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!I2:I100, ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num)),
-        _xlpm.Jcol, _xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!J2:J100, ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num)),
-        _xlpm.Kcol, _xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!K2:K100, ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num)),
-        _xlpm.transactions, IF(ROWS(_xlpm.filtered_txns)&gt;0,
-          _xlfn.TEXTJOIN(CHAR(10), TRUE, _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.filtered_txns)), _xlfn.LAMBDA(_xlpm.i,
-            "&lt;tr&gt;&lt;td&gt;" &amp;
-            IF(INDEX(_xlpm.Fcol, _xlpm.i)="Y",
-"&lt;Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 1) &amp; "&lt;/Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;",
-"&lt;Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 1) &amp; "&lt;/Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;"
-            )
-             &amp;
-            "&lt;/td&gt;&lt;td&gt;" &amp;
-            IF(INDEX(_xlpm.Fcol, _xlpm.i)="Y",
-"&lt;Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 2) &amp; "&lt;/Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;",
-"&lt;Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 2) &amp; "&lt;/Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;"
-            )
-             &amp;
-            "&lt;/td&gt;&lt;td&gt;" &amp;
-            "&lt;Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_Bank&gt;" &amp; INDEX(_xlpm.Jcol, _xlpm.i) &amp; "&lt;/Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_Bank&gt;" &amp; " " &amp; "&lt;Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_AccountNumber&gt;" &amp; INDEX(_xlpm.Kcol, _xlpm.i) &amp; "&lt;/Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_AccountNumber&gt;"
-             &amp;
-            "&lt;/td&gt;&lt;/tr&gt;"
-          ))),
-          "&lt;tr&gt;&lt;td colspan='3'&gt;No Transaction&lt;/td&gt;&lt;/tr&gt;"
+        _xlpm.filter_condition, ('PoliceLetter-Txn-Details'!A2:A100 &lt;&gt; "") * ('PoliceLetter-Txn-Details'!G2:G100 = _xlpm.suspect_num),
+        _xlpm.filtered_txns, IFERROR(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!B2:D100, _xlpm.filter_condition), ""),
+        _xlpm.Ecol, IFERROR(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!E2:E100, _xlpm.filter_condition), ""),
+        _xlpm.Fcol, IFERROR(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!F2:F100, _xlpm.filter_condition), ""),
+        _xlpm.Hcol, IFERROR(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!H2:H100, _xlpm.filter_condition), ""),
+        _xlpm.Icol, IFERROR(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!I2:I100, _xlpm.filter_condition), ""),
+        _xlpm.Jcol, IFERROR(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!J2:J100, _xlpm.filter_condition), ""),
+        _xlpm.Kcol, IFERROR(_xlfn._xlws.FILTER('PoliceLetter-Txn-Details'!K2:K100, _xlpm.filter_condition), ""),
+        _xlpm.transactions, IF(AND(ISTEXT(_xlpm.filtered_txns), _xlpm.filtered_txns=""),
+          "&lt;tr&gt;&lt;td colspan='3'&gt;No Transaction&lt;/td&gt;&lt;/tr&gt;",
+          IF(ROWS(_xlpm.filtered_txns)&gt;0,
+            _xlfn.TEXTJOIN(CHAR(10), TRUE, _xlfn.MAP(_xlfn.SEQUENCE(ROWS(_xlpm.filtered_txns)), _xlfn.LAMBDA(_xlpm.i,
+              "&lt;tr&gt;&lt;td&gt;" &amp;
+              IF(INDEX(_xlpm.Fcol, _xlpm.i)="Y",
+  "&lt;Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 1) &amp; "&lt;/Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;",
+  "&lt;Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 1) &amp; "&lt;/Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Date&gt;"
+              )
+               &amp;
+              "&lt;/td&gt;&lt;td&gt;" &amp;
+              IF(INDEX(_xlpm.Fcol, _xlpm.i)="Y",
+  "&lt;Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 2) &amp; "&lt;/Template_Located_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;",
+  "&lt;Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;" &amp; INDEX(_xlpm.filtered_txns, _xlpm.i, 2) &amp; "&lt;/Template_NotLocated_FraudPayment"&amp;INDEX(_xlpm.Ecol, _xlpm.i)&amp;"_Amount&gt;"
+              )
+               &amp;
+              "&lt;/td&gt;&lt;td&gt;" &amp;
+              "&lt;Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_Bank&gt;" &amp; INDEX(_xlpm.Jcol, _xlpm.i) &amp; "&lt;/Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_Bank&gt;" &amp; " " &amp; "&lt;Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_AccountNumber&gt;" &amp; INDEX(_xlpm.Kcol, _xlpm.i) &amp; "&lt;/Template_Victim"&amp;INDEX(_xlpm.Hcol, _xlpm.i)&amp;"_Account"&amp;INDEX(_xlpm.Icol, _xlpm.i)&amp;"_AccountNumber&gt;"
+               &amp;
+              "&lt;/td&gt;&lt;/tr&gt;"
+            ))),
+            "&lt;tr&gt;&lt;td colspan='3'&gt;No Transaction&lt;/td&gt;&lt;/tr&gt;"
+          )
         ),
         _xlfn.TEXTJOIN(CHAR(10), TRUE, _xlpm.header, _xlpm.transactions)
       ),
@@ -1668,7 +1625,7 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment1=7_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Amount&gt;100000&lt;/Template_Located_FraudPayment1=7_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment1=7_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Amount&gt;100000&lt;/Template_Located_FraudPayment1=7_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could
@@ -1684,8 +1641,8 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment2=8_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Amount&gt;100000&lt;/Template_Located_FraudPayment2=8_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment3=9_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Amount&gt;100000&lt;/Template_Located_FraudPayment3=9_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment2=8_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Amount&gt;100000&lt;/Template_Located_FraudPayment2=8_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment3=9_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Amount&gt;100000&lt;/Template_Located_FraudPayment3=9_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could
@@ -1701,8 +1658,8 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment10_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Amount&gt;100000&lt;/Template_Located_FraudPayment10_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment4=11_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Amount&gt;100000&lt;/Template_Located_FraudPayment4=11_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment10_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Amount&gt;100000&lt;/Template_Located_FraudPayment10_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment4=11_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Amount&gt;100000&lt;/Template_Located_FraudPayment4=11_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could
@@ -1718,7 +1675,7 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment5+6_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Amount&gt;100000&lt;/Template_Located_FraudPayment5+6_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment5+6_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Amount&gt;100000&lt;/Template_Located_FraudPayment5+6_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could
@@ -1730,7 +1687,7 @@
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
+      <c r="B10" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2036,8 +1993,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96EC2D32-9E76-C94A-A5ED-4395688F3423}">
   <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection sqref="A1:A41"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2081,7 +2038,7 @@
         <v>*Fax:* 282■■■■■</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'PoliceLetter-Runtime-Params'!B1</f>
         <v>&lt;Template_PoliceInvestigationTeam&gt;District Investigation Team 7&lt;/Template_PoliceInvestigationTeam&gt;
@@ -2130,7 +2087,7 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment1=7_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Amount&gt;100000&lt;/Template_Located_FraudPayment1=7_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment1=7_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment1=7_Amount&gt;100000&lt;/Template_Located_FraudPayment1=7_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could
@@ -2146,8 +2103,8 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment2=8_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Amount&gt;100000&lt;/Template_Located_FraudPayment2=8_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment3=9_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Amount&gt;100000&lt;/Template_Located_FraudPayment3=9_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment2=8_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment2=8_Amount&gt;100000&lt;/Template_Located_FraudPayment2=8_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment3=9_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment3=9_Amount&gt;100000&lt;/Template_Located_FraudPayment3=9_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could
@@ -2163,8 +2120,8 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment10_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Amount&gt;100000&lt;/Template_Located_FraudPayment10_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment4=11_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Amount&gt;100000&lt;/Template_Located_FraudPayment4=11_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment10_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment10_Amount&gt;100000&lt;/Template_Located_FraudPayment10_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Date&gt;2024-12-31&lt;/Template_Located_FraudPayment4=11_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment4=11_Amount&gt;100000&lt;/Template_Located_FraudPayment4=11_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could
@@ -2180,7 +2137,7 @@
 &lt;tr&gt;&lt;th colspan='3'&gt;Suspected nature of transactions:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Might have been used in receicing proceeds of crime&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Might have been used to receive funds related to terrorist financing&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Exhibited transaction patterns which were incommensurate with holder's background&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;If the predicate offence is deception related, please state the type of deception:&lt;/th&gt;&lt;tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Telephone Deception&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] E-shopping Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Romance Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [X] Investment Scam&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Employment Fraud&lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt; - [ ] Others (please specify) &lt;/td&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;(please tick if appropriate)&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Transaction Details:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;th&gt;Date&lt;/th&gt;&lt;th&gt;Amount&lt;/th&gt;&lt;th&gt;Transferor's Bank and Account&lt;/th&gt;&lt;/tr&gt;
-&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment5+6_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Amount&gt;100000&lt;/Template_Located_FraudPayment5+6_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim_Account_Bank&gt;Cash&lt;/Template_Victim_Account_Bank&gt; &lt;Template_Victim_Account_AccountNumber&gt;Cash&lt;/Template_Victim_Account_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
+&lt;tr&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Date&gt;2024-12-30&lt;/Template_Located_FraudPayment5+6_Date&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Located_FraudPayment5+6_Amount&gt;100000&lt;/Template_Located_FraudPayment5+6_Amount&gt;&lt;/td&gt;&lt;td&gt;&lt;Template_Victim0_Account0_Bank&gt;Cash&lt;/Template_Victim0_Account0_Bank&gt; &lt;Template_Victim0_Account0_AccountNumber&gt;Cash&lt;/Template_Victim0_Account0_AccountNumber&gt;&lt;/td&gt;&lt;/tr&gt;
 &lt;tr&gt;&lt;th colspan='3'&gt;Case Summary:&lt;/th&gt;&lt;/tr&gt;&lt;tr&gt;&lt;td colspan='3'&gt;On 2025-01-03, a female reported to police that between 2024-12-18 and 2024-12-31, she
 was lured to invest into forex trading and had deposited a total of HK$1,149,000 into 11
 bank accounts (including the above listed transactions). The female later found she could

</xml_diff>